<commit_message>
revisi generate id zona patroli dan jadwal patroli
</commit_message>
<xml_diff>
--- a/assets/path_upload/upload_checkpoint_.xlsx
+++ b/assets/path_upload/upload_checkpoint_.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="48">
   <si>
     <t>ID CHECKPOINT</t>
   </si>
@@ -31,25 +31,133 @@
     <t>INSTALASI</t>
   </si>
   <si>
-    <t>DURASI BATAS ATAS</t>
-  </si>
-  <si>
-    <t>DURASI BATAS BAWAH</t>
+    <t>PLANT 5</t>
+  </si>
+  <si>
+    <t>CRITICAL AREA</t>
+  </si>
+  <si>
+    <t>Critical Area_Substation Welding</t>
+  </si>
+  <si>
+    <t>Critical Area_POM mini Quality / Audit</t>
+  </si>
+  <si>
+    <t>Critical Area_Substation Assy</t>
+  </si>
+  <si>
+    <t>Critical Area_Pertamax</t>
+  </si>
+  <si>
+    <t>Critical Area_Substation RND / Gardu PLN</t>
+  </si>
+  <si>
+    <t>Critical Area_Cooling tower  RnD</t>
+  </si>
+  <si>
+    <t>Critical Area_Solar / Genset</t>
+  </si>
+  <si>
+    <t>Critical Area_Samator / TPS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FACTORY </t>
+  </si>
+  <si>
+    <t>Factory_Press Utara</t>
+  </si>
+  <si>
+    <t>Factory_Press Selatan</t>
+  </si>
+  <si>
+    <t>Factory_ Welding Office CKD</t>
+  </si>
+  <si>
+    <t>Factory_Assembling Office Log</t>
+  </si>
+  <si>
+    <t>Factory_Assembling Benchtry</t>
+  </si>
+  <si>
+    <t>OFFICE</t>
+  </si>
+  <si>
+    <t>Office_Central Office Lantai 1</t>
+  </si>
+  <si>
+    <t>Office_Central Office lantai 2</t>
+  </si>
+  <si>
+    <t>Office_RND Engineering</t>
+  </si>
+  <si>
+    <t>Office_RND Design</t>
   </si>
   <si>
     <t>PARIMETER</t>
   </si>
   <si>
-    <t>PLANT 5</t>
+    <t>Parimeter_Pos 3</t>
+  </si>
+  <si>
+    <t>Parimeter_Pos 2</t>
+  </si>
+  <si>
+    <t>Parimeter_Pos 1</t>
+  </si>
+  <si>
+    <t>Parimeter_Paddock</t>
+  </si>
+  <si>
+    <t>Parimeter_Perbatasan AI / Soil Road</t>
+  </si>
+  <si>
+    <t>FASUM</t>
+  </si>
+  <si>
+    <t>Fasum_Loker Karyawan</t>
+  </si>
+  <si>
+    <t>Fasum_Klinik, FM, kantin, &amp; Rest Area</t>
+  </si>
+  <si>
+    <t>Fasum_Area parkiran KR2 &amp; Kr4</t>
+  </si>
+  <si>
+    <t>Fasum_KEC</t>
+  </si>
+  <si>
+    <t>ADMP5CRI</t>
+  </si>
+  <si>
+    <t>ADMP5FAC</t>
+  </si>
+  <si>
+    <t>ADMP5OFC</t>
   </si>
   <si>
     <t>ADMP5PAR</t>
   </si>
   <si>
-    <t>PARIMETER_CKD PPL1</t>
-  </si>
-  <si>
-    <t>PARIMETER_Inbound PPL1</t>
+    <t>ADMP5FAS</t>
+  </si>
+  <si>
+    <t>Critical Area_Substation Press</t>
+  </si>
+  <si>
+    <t>Parimeter_Menara 2</t>
+  </si>
+  <si>
+    <t>Parimeter_Jalan Baru</t>
+  </si>
+  <si>
+    <t>FACTORY</t>
+  </si>
+  <si>
+    <t>Durasi Batas Atas</t>
+  </si>
+  <si>
+    <t>Durasi Batas Bawah</t>
   </si>
 </sst>
 </file>
@@ -59,7 +167,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,6 +190,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF212529"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -97,7 +220,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -120,21 +243,51 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Currency [0]" xfId="1" builtinId="7"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -433,10 +586,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -445,16 +598,16 @@
     <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
     <col min="4" max="4" width="21.140625" customWidth="1"/>
-    <col min="5" max="5" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="6" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -467,56 +620,677 @@
         <v>1</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>6</v>
       </c>
       <c r="D2" s="3">
-        <v>3898987838344</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="4">
-        <v>10</v>
-      </c>
-      <c r="G2" s="4">
-        <v>5</v>
+        <v>2878134531</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" s="13">
+        <v>0</v>
+      </c>
+      <c r="G2" s="13">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="3">
+        <v>2878900771</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="13">
+        <v>0</v>
+      </c>
+      <c r="G3" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="3">
+        <v>2878815507</v>
+      </c>
+      <c r="E4" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="F4" s="13">
+        <v>0</v>
+      </c>
+      <c r="G4" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="3">
+        <v>2879083011</v>
+      </c>
+      <c r="E5" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="3">
-        <v>3898987838345</v>
-      </c>
-      <c r="E3" s="4" t="s">
+      <c r="F5" s="13">
+        <v>0</v>
+      </c>
+      <c r="G5" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="3">
+        <v>2878646435</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="13">
+        <v>0</v>
+      </c>
+      <c r="G6" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="3">
+        <v>2879251363</v>
+      </c>
+      <c r="E7" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="4">
-        <v>10</v>
-      </c>
-      <c r="G3" s="4">
-        <v>5</v>
+      <c r="F7" s="13">
+        <v>0</v>
+      </c>
+      <c r="G7" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="3">
+        <v>2877126179</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="13">
+        <v>0</v>
+      </c>
+      <c r="G8" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="3">
+        <v>2878061763</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="13">
+        <v>0</v>
+      </c>
+      <c r="G9" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="3">
+        <v>2879215987</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="13">
+        <v>0</v>
+      </c>
+      <c r="G10" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="3">
+        <v>2878695475</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="13">
+        <v>0</v>
+      </c>
+      <c r="G11" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="3">
+        <v>2877511171</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="13">
+        <v>0</v>
+      </c>
+      <c r="G12" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="3">
+        <v>2879259539</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="13">
+        <v>0</v>
+      </c>
+      <c r="G13" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="3">
+        <v>2870908115</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="13">
+        <v>0</v>
+      </c>
+      <c r="G14" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="3">
+        <v>2878814995</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" s="13">
+        <v>0</v>
+      </c>
+      <c r="G15" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="3">
+        <v>2878381459</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F16" s="13">
+        <v>0</v>
+      </c>
+      <c r="G16" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="3">
+        <v>2877860963</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F17" s="13">
+        <v>0</v>
+      </c>
+      <c r="G17" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="3">
+        <v>2878172995</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" s="13">
+        <v>0</v>
+      </c>
+      <c r="G18" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="3">
+        <v>2878044851</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F19" s="13">
+        <v>0</v>
+      </c>
+      <c r="G19" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" s="3">
+        <v>2878044579</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F20" s="13">
+        <v>0</v>
+      </c>
+      <c r="G20" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="3">
+        <v>2878290899</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F21" s="13">
+        <v>0</v>
+      </c>
+      <c r="G21" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="3">
+        <v>2878027971</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F22" s="13">
+        <v>0</v>
+      </c>
+      <c r="G22" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D23" s="3">
+        <v>2877314771</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F23" s="13">
+        <v>0</v>
+      </c>
+      <c r="G23" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D24" s="3">
+        <v>2862662003</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F24" s="13">
+        <v>0</v>
+      </c>
+      <c r="G24" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25" s="3">
+        <v>2879107315</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F25" s="13">
+        <v>0</v>
+      </c>
+      <c r="G25" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26" s="3">
+        <v>2877996899</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F26" s="13">
+        <v>0</v>
+      </c>
+      <c r="G26" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27" s="3">
+        <v>2862239795</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F27" s="13">
+        <v>0</v>
+      </c>
+      <c r="G27" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D28" s="3">
+        <v>2877692131</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F28" s="13">
+        <v>0</v>
+      </c>
+      <c r="G28" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D29" s="3">
+        <v>2878953811</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F29" s="13">
+        <v>0</v>
+      </c>
+      <c r="G29" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D30" s="3">
+        <v>2878502787</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F30" s="13">
+        <v>0</v>
+      </c>
+      <c r="G30" s="13">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>